<commit_message>
feat(hunter): add access denied logs + file management
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hadibereksi/Documents/Epitech/TEK5/Extia/sideProject/GoPassHunt/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F32D35B2-61DE-FF48-A0E7-88D74C0F0926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED08D942-4A21-EE4E-BDBF-8225F0A45A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{C5F990E7-7D44-5840-8240-85E7DA7FBC8A}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{C5F990E7-7D44-5840-8240-85E7DA7FBC8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>first name</t>
   </si>
@@ -70,6 +72,18 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>Theo</t>
+  </si>
+  <si>
+    <t>los pollos</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>mot de passe</t>
   </si>
 </sst>
 </file>
@@ -434,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12F95FD-AB62-BA44-B94B-DF001C48597D}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,4 +512,144 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD143201-1EE6-514F-ADE0-9B926A43667E}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5CF20FAE-CE5E-344A-A66A-5D510FB09718}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{C84D5A5F-726A-8348-ADF2-1BEBAF73F7DB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8181DE30-AE4E-0F45-B934-E7568527A92D}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6282890C-5F19-A549-B522-105C4D099FD4}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{17B621EF-0E47-9841-AAD4-496B9AE0C5F4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>